<commit_message>
presun do slozek, pridan check pro kopirovatelny vzorec
</commit_message>
<xml_diff>
--- a/23_fb750.xlsx
+++ b/23_fb750.xlsx
@@ -8,15 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/Projekty/bakalářská-práce/BP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F4FE6B-1850-6845-951E-5736C668DACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE10C966-5841-5840-9211-77BAB241143D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2140" yWindow="-21000" windowWidth="38400" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2140" yWindow="-21000" windowWidth="38400" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="zdroj" sheetId="2" r:id="rId1"/>
     <sheet name="data" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -411,7 +424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD9DDF49-B077-3A47-B8DB-141441FA9A60}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
@@ -423,8 +436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
definovany nazev pole misto adresy
</commit_message>
<xml_diff>
--- a/23_fb750.xlsx
+++ b/23_fb750.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/Projekty/bakalářská-práce/BP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F43C9B5-4BF1-D541-972E-6DA69635783F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58DFAC42-AAB4-A947-AA66-D3620A4CACF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="34200" windowHeight="21460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="zdroj" sheetId="2" r:id="rId1"/>
     <sheet name="data" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="pole">data!$E$30</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,28 +34,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -464,10 +445,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -481,7 +462,7 @@
     <col min="12" max="12" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -501,7 +482,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -519,13 +500,13 @@
         <v>22.169988904709889</v>
       </c>
       <c r="F2" s="1" t="str">
-        <f>IF(E$30&gt;E2,"ne","více")</f>
+        <f>IF(pole&gt;E2,"ne","více")</f>
         <v>ne</v>
       </c>
       <c r="G2" s="1"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -547,18 +528,10 @@
         <v>více</v>
       </c>
       <c r="I3" s="3"/>
-      <c r="J3" s="3">
-        <v>100</v>
-      </c>
-      <c r="K3" s="3">
-        <v>11</v>
-      </c>
-      <c r="L3" cm="1">
-        <f t="array" ref="L3:L5">J3:J5-K3:K5</f>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -580,17 +553,10 @@
         <v>ne</v>
       </c>
       <c r="I4" s="3"/>
-      <c r="J4" s="3">
-        <v>200</v>
-      </c>
-      <c r="K4" s="3">
-        <v>12</v>
-      </c>
-      <c r="L4">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -612,17 +578,10 @@
         <v>více</v>
       </c>
       <c r="I5" s="3"/>
-      <c r="J5" s="3">
-        <v>300</v>
-      </c>
-      <c r="K5" s="3">
-        <v>13</v>
-      </c>
-      <c r="L5">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -646,7 +605,7 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -670,7 +629,7 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -692,7 +651,7 @@
         <v>ne</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -714,7 +673,7 @@
         <v>ne</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -736,7 +695,7 @@
         <v>více</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -758,7 +717,7 @@
         <v>ne</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -780,7 +739,7 @@
         <v>více</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -802,7 +761,7 @@
         <v>ne</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -824,7 +783,7 @@
         <v>více</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -846,7 +805,7 @@
         <v>více</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
chybi jednotlive popisne charakteristiky
</commit_message>
<xml_diff>
--- a/23_fb750.xlsx
+++ b/23_fb750.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/Projekty/bakalářská-práce/BP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF706F7-4E4D-4D4F-890D-AEA3FE288411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0954EEFF-894B-5B44-A7EB-E6040AE026F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="34200" windowHeight="21460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -455,7 +455,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
komentare a uprava podmineneho formatovani
</commit_message>
<xml_diff>
--- a/23_fb750.xlsx
+++ b/23_fb750.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/Projekty/bakalářská-práce/BP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31490ED1-E0E0-4041-984D-D7368A7CED3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E030AD-42CB-7D49-A0A7-5C8050185201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="34200" windowHeight="21460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -88,13 +88,20 @@
   <numFmts count="1">
     <numFmt numFmtId="171" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -279,15 +286,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="171" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -303,19 +301,91 @@
     </xf>
     <xf numFmtId="171" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="4" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -630,7 +700,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+      <selection activeCell="E2" sqref="E2:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -639,33 +709,33 @@
     <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
     <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="23" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="9">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -681,7 +751,7 @@
         <f>D2/(C2/100)^2</f>
         <v>22.169988904709889</v>
       </c>
-      <c r="F2" s="10" t="str">
+      <c r="F2" s="7" t="str">
         <f>IF(E$30&gt;E2,"ne","více")</f>
         <v>ne</v>
       </c>
@@ -689,7 +759,7 @@
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="9">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -705,7 +775,7 @@
         <f t="shared" ref="E3:E22" si="0">D3/(C3/100)^2</f>
         <v>40.609272228583599</v>
       </c>
-      <c r="F3" s="10" t="str">
+      <c r="F3" s="7" t="str">
         <f t="shared" ref="F3:F23" si="1">IF(E$30&gt;E3,"ne","více")</f>
         <v>více</v>
       </c>
@@ -714,7 +784,7 @@
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="9">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -730,7 +800,7 @@
         <f t="shared" si="0"/>
         <v>20.194670685802109</v>
       </c>
-      <c r="F4" s="10" t="str">
+      <c r="F4" s="7" t="str">
         <f t="shared" si="1"/>
         <v>ne</v>
       </c>
@@ -739,7 +809,7 @@
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="9">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -755,7 +825,7 @@
         <f t="shared" si="0"/>
         <v>36.520207581818859</v>
       </c>
-      <c r="F5" s="10" t="str">
+      <c r="F5" s="7" t="str">
         <f t="shared" si="1"/>
         <v>více</v>
       </c>
@@ -764,7 +834,7 @@
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="9">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -780,7 +850,7 @@
         <f t="shared" si="0"/>
         <v>18.998630788332839</v>
       </c>
-      <c r="F6" s="10" t="str">
+      <c r="F6" s="7" t="str">
         <f t="shared" si="1"/>
         <v>ne</v>
       </c>
@@ -788,7 +858,7 @@
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="9">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -804,7 +874,7 @@
         <f t="shared" si="0"/>
         <v>25.338325253924282</v>
       </c>
-      <c r="F7" s="10" t="str">
+      <c r="F7" s="7" t="str">
         <f t="shared" si="1"/>
         <v>ne</v>
       </c>
@@ -812,7 +882,7 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="9">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -828,13 +898,13 @@
         <f t="shared" si="0"/>
         <v>24.040864408259427</v>
       </c>
-      <c r="F8" s="10" t="str">
+      <c r="F8" s="7" t="str">
         <f t="shared" si="1"/>
         <v>ne</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="9">
+      <c r="A9" s="6">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -850,13 +920,13 @@
         <f t="shared" si="0"/>
         <v>27.122389574320355</v>
       </c>
-      <c r="F9" s="10" t="str">
+      <c r="F9" s="7" t="str">
         <f t="shared" si="1"/>
         <v>ne</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -872,13 +942,13 @@
         <f t="shared" si="0"/>
         <v>35.963891819747673</v>
       </c>
-      <c r="F10" s="10" t="str">
+      <c r="F10" s="7" t="str">
         <f t="shared" si="1"/>
         <v>více</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="9">
+      <c r="A11" s="6">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -894,13 +964,13 @@
         <f t="shared" si="0"/>
         <v>21.750626929835043</v>
       </c>
-      <c r="F11" s="10" t="str">
+      <c r="F11" s="7" t="str">
         <f t="shared" si="1"/>
         <v>ne</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="9">
+      <c r="A12" s="6">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -916,13 +986,13 @@
         <f t="shared" si="0"/>
         <v>38.937797430362174</v>
       </c>
-      <c r="F12" s="10" t="str">
+      <c r="F12" s="7" t="str">
         <f t="shared" si="1"/>
         <v>více</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="9">
+      <c r="A13" s="6">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -938,13 +1008,13 @@
         <f t="shared" si="0"/>
         <v>25.060881057152045</v>
       </c>
-      <c r="F13" s="10" t="str">
+      <c r="F13" s="7" t="str">
         <f t="shared" si="1"/>
         <v>ne</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="9">
+      <c r="A14" s="6">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -960,13 +1030,13 @@
         <f t="shared" si="0"/>
         <v>32.8772876754065</v>
       </c>
-      <c r="F14" s="10" t="str">
+      <c r="F14" s="7" t="str">
         <f t="shared" si="1"/>
         <v>více</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="9">
+      <c r="A15" s="6">
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -982,13 +1052,13 @@
         <f t="shared" si="0"/>
         <v>39.195778105615709</v>
       </c>
-      <c r="F15" s="10" t="str">
+      <c r="F15" s="7" t="str">
         <f t="shared" si="1"/>
         <v>více</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="9">
+      <c r="A16" s="6">
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -1004,13 +1074,13 @@
         <f t="shared" si="0"/>
         <v>38.541898334112503</v>
       </c>
-      <c r="F16" s="10" t="str">
+      <c r="F16" s="7" t="str">
         <f t="shared" si="1"/>
         <v>více</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="9">
+      <c r="A17" s="6">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -1026,13 +1096,13 @@
         <f t="shared" si="0"/>
         <v>40.522655178326467</v>
       </c>
-      <c r="F17" s="10" t="str">
+      <c r="F17" s="7" t="str">
         <f t="shared" si="1"/>
         <v>více</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="9">
+      <c r="A18" s="6">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -1048,13 +1118,13 @@
         <f t="shared" si="0"/>
         <v>29.405035554757085</v>
       </c>
-      <c r="F18" s="10" t="str">
+      <c r="F18" s="7" t="str">
         <f t="shared" si="1"/>
         <v>ne</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="9">
+      <c r="A19" s="6">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -1070,13 +1140,13 @@
         <f t="shared" si="0"/>
         <v>31.30683726346486</v>
       </c>
-      <c r="F19" s="10" t="str">
+      <c r="F19" s="7" t="str">
         <f t="shared" si="1"/>
         <v>více</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="9">
+      <c r="A20" s="6">
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -1092,13 +1162,13 @@
         <f t="shared" si="0"/>
         <v>45.06786690545762</v>
       </c>
-      <c r="F20" s="10" t="str">
+      <c r="F20" s="7" t="str">
         <f t="shared" si="1"/>
         <v>více</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="9">
+      <c r="A21" s="6">
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -1114,13 +1184,13 @@
         <f t="shared" si="0"/>
         <v>24.87273119569911</v>
       </c>
-      <c r="F21" s="10" t="str">
+      <c r="F21" s="7" t="str">
         <f t="shared" si="1"/>
         <v>ne</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="9">
+      <c r="A22" s="6">
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1136,87 +1206,87 @@
         <f t="shared" si="0"/>
         <v>30.765402404662261</v>
       </c>
-      <c r="F22" s="10" t="str">
+      <c r="F22" s="7" t="str">
         <f t="shared" si="1"/>
         <v>ne</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="11">
+      <c r="A23" s="8">
         <v>22</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="10">
         <v>174.5</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="10">
         <v>126.9</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23" s="11">
         <f>D23/(C23/100)^2</f>
         <v>41.674534691833401</v>
       </c>
-      <c r="F23" s="15" t="str">
+      <c r="F23" s="12" t="str">
         <f t="shared" si="1"/>
         <v>více</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="17"/>
-      <c r="B27" s="7" t="s">
+      <c r="A27" s="14"/>
+      <c r="B27" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="18" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="16">
+      <c r="B28" s="13">
         <f>MIN(C2:C23)</f>
         <v>158.1</v>
       </c>
-      <c r="C28" s="16">
+      <c r="C28" s="13">
         <f>MAX(C2:C23)</f>
         <v>189.6</v>
       </c>
-      <c r="D28" s="16">
+      <c r="D28" s="13">
         <f>AVERAGE(C2:C23)</f>
         <v>171.55454545454543</v>
       </c>
-      <c r="E28" s="19">
+      <c r="E28" s="21">
         <f>MEDIAN(C2:C23)</f>
         <v>171.75</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="16">
+      <c r="B29" s="13">
         <f>MIN(D2:D23)</f>
         <v>55.1</v>
       </c>
-      <c r="C29" s="16">
+      <c r="C29" s="13">
         <f>MAX(D2:D23)</f>
         <v>126.9</v>
       </c>
-      <c r="D29" s="16">
+      <c r="D29" s="13">
         <f>AVERAGE(D2:D23)</f>
         <v>91.954545454545482</v>
       </c>
-      <c r="E29" s="19">
+      <c r="E29" s="21">
         <f>MEDIAN(D2:D23)</f>
         <v>94.45</v>
       </c>
@@ -1225,24 +1295,35 @@
       <c r="A30" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="21">
+      <c r="B30" s="15">
         <f>MIN(E2:E23)</f>
         <v>18.998630788332839</v>
       </c>
-      <c r="C30" s="22">
+      <c r="C30" s="15">
         <f>MAX(E2:E23)</f>
         <v>45.06786690545762</v>
       </c>
-      <c r="D30" s="22">
+      <c r="D30" s="15">
         <f>AVERAGE(E2:E23)</f>
         <v>31.406253362371999</v>
       </c>
-      <c r="E30" s="23">
+      <c r="E30" s="22">
         <f>MEDIAN(E2:E23)</f>
         <v>31.036119834063562</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E2:E23">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+      <formula>25</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+      <formula>18</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+      <formula>18.5</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>

<commit_message>
kontrola pro existujici graf
</commit_message>
<xml_diff>
--- a/23_fb750.xlsx
+++ b/23_fb750.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/Projekty/bakalářská-práce/BP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFC659C-3229-2B45-8270-807AE818372E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2078D138-3807-F144-926D-0B406E412B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="34200" windowHeight="21460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="data" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">data!$D$2:$D$23</definedName>
     <definedName name="pole">data!$E$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -601,6 +602,900 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="cs-CZ"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="cs-CZ"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$D$2:$D$23</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>64.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>103.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>91.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>55.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>84.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>99.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>56.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>121.3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>75.7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>114.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>110.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>101.9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>76.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>104.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>122.4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>74.7</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>76.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>126.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A159-3D42-A79D-DE06E1825D23}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="463310784"/>
+        <c:axId val="463312576"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="463310784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="463312576"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="463312576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="463310784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="cs-CZ"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>148167</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>110066</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>275167</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graf 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BA8FAFD-6EFB-E2F2-EEF6-39651AC67E1D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -905,7 +1800,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1528,5 +2423,6 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
pridana cast kontrol pro calc
</commit_message>
<xml_diff>
--- a/23_fb750.xlsx
+++ b/23_fb750.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/Projekty/bakalářská-práce/BP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180BCD1E-D0DF-2045-8C96-EAF48C9F215B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59FDE39-CA4F-6243-835B-37373D897AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="34200" windowHeight="21460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,6 +20,7 @@
     <definedName name="_xlchart.v1.0" hidden="1">data!$D$2:$D$23</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">data!$D$2:$D$23</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">data!$D$2:$D$23</definedName>
+    <definedName name="hodnota">data!$E$28</definedName>
     <definedName name="pole">data!$E$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -278,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -324,11 +325,58 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="40">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1660,16 +1708,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>148167</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>110066</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>402167</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>275167</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>592667</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1999,7 +2047,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="E3" sqref="E3:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2104,7 +2152,7 @@
         <v>ne</v>
       </c>
       <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="J4" s="25"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -2311,6 +2359,7 @@
         <f t="shared" si="1"/>
         <v>ne</v>
       </c>
+      <c r="K13" s="26"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
@@ -2462,7 +2511,7 @@
         <v>45.06786690545762</v>
       </c>
       <c r="F20" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(E$30&gt;E20,"ne","více")</f>
         <v>více</v>
       </c>
     </row>
@@ -2612,12 +2661,12 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E23">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
+  <conditionalFormatting sqref="E3:E23">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+      <formula>25</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>18.5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="greaterThan">
-      <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
pridany checky pro calc a upraveny pro excel aby bylo vse jednote
</commit_message>
<xml_diff>
--- a/23_fb750.xlsx
+++ b/23_fb750.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/Projekty/bakalářská-práce/BP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59FDE39-CA4F-6243-835B-37373D897AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFE4C72-1ACB-704E-AA75-A23145BDC79A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="34200" windowHeight="21460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,6 +20,9 @@
     <definedName name="_xlchart.v1.0" hidden="1">data!$D$2:$D$23</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">data!$D$2:$D$23</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">data!$D$2:$D$23</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">data!$D$2:$D$23</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">data!$D$2:$D$23</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">data!$D$2:$D$23</definedName>
     <definedName name="hodnota">data!$E$28</definedName>
     <definedName name="pole">data!$E$30</definedName>
   </definedNames>
@@ -279,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -321,12 +324,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -779,6 +786,7 @@
                 <a:endParaRPr lang="cs-CZ"/>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -888,6 +896,7 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -1708,16 +1717,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>402167</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>31751</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>46565</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>592667</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>158751</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>112182</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2047,7 +2056,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E23"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2077,7 +2086,7 @@
       <c r="E1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="27" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2094,7 +2103,7 @@
       <c r="D2" s="4">
         <v>64.599999999999994</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="28">
         <f>D2/(C2/100)^2</f>
         <v>22.169988904709889</v>
       </c>
@@ -2225,7 +2234,7 @@
         <f t="shared" si="1"/>
         <v>ne</v>
       </c>
-      <c r="I7" s="1"/>
+      <c r="I7" s="23"/>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
pridan abstraktni spredsheet, uprava get_cell_style u exceliu
</commit_message>
<xml_diff>
--- a/23_fb750.xlsx
+++ b/23_fb750.xlsx
@@ -8,21 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/Projekty/bakalářská-práce/BP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFE4C72-1ACB-704E-AA75-A23145BDC79A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80079573-5377-FA4F-A7A0-A0C67F51DEC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="34200" windowHeight="21460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="34200" windowHeight="19860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="zdroj" sheetId="2" r:id="rId1"/>
     <sheet name="data" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">data!$D$2:$D$23</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">data!$D$2:$D$23</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">data!$D$2:$D$23</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">data!$D$2:$D$23</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">data!$D$2:$D$23</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">data!$D$2:$D$23</definedName>
     <definedName name="hodnota">data!$E$28</definedName>
     <definedName name="pole">data!$E$30</definedName>
   </definedNames>
@@ -282,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -327,18 +321,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -353,296 +345,6 @@
       <font>
         <color rgb="FF9C0006"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -2056,7 +1758,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2086,7 +1788,7 @@
       <c r="E1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="26" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2103,7 +1805,7 @@
       <c r="D2" s="4">
         <v>64.599999999999994</v>
       </c>
-      <c r="E2" s="28">
+      <c r="E2" s="5">
         <f>D2/(C2/100)^2</f>
         <v>22.169988904709889</v>
       </c>
@@ -2161,7 +1863,7 @@
         <v>ne</v>
       </c>
       <c r="I4" s="1"/>
-      <c r="J4" s="25"/>
+      <c r="J4" s="24"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -2211,7 +1913,7 @@
         <v>ne</v>
       </c>
       <c r="I6" s="1"/>
-      <c r="J6" s="24"/>
+      <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
@@ -2368,7 +2070,7 @@
         <f t="shared" si="1"/>
         <v>ne</v>
       </c>
-      <c r="K13" s="26"/>
+      <c r="K13" s="25"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
@@ -2671,11 +2373,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E3:E23">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
-      <formula>25</formula>
-    </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>18.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+      <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>